<commit_message>
nav bar and state fixes
</commit_message>
<xml_diff>
--- a/data/master.xlsx
+++ b/data/master.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="112">
   <si>
     <t>County</t>
   </si>
@@ -177,6 +177,9 @@
     <t>Use portal or email clerk</t>
   </si>
   <si>
+    <t>2025-08-11</t>
+  </si>
+  <si>
     <t>Fort Myers</t>
   </si>
   <si>
@@ -192,15 +195,27 @@
     <t>Use portal + All-in-one email</t>
   </si>
   <si>
+    <t>2025-08-12</t>
+  </si>
+  <si>
     <t>Fort Myers Planning Department</t>
   </si>
   <si>
+    <t>2025-08-13</t>
+  </si>
+  <si>
     <t>Fort Myers Environmental Department</t>
   </si>
   <si>
+    <t>2025-08-14</t>
+  </si>
+  <si>
     <t>Fort Myers Fire Department</t>
   </si>
   <si>
+    <t>2025-08-15</t>
+  </si>
+  <si>
     <t>Monroe</t>
   </si>
   <si>
@@ -216,15 +231,27 @@
     <t>https://monroecountyfl.nextrequest.com/</t>
   </si>
   <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
     <t>Monroe County Planning Department</t>
   </si>
   <si>
+    <t>2025-08-17</t>
+  </si>
+  <si>
     <t>Monroe County Environmental Department</t>
   </si>
   <si>
+    <t>2025-08-18</t>
+  </si>
+  <si>
     <t>Monroe County Fire Department</t>
   </si>
   <si>
+    <t>2025-08-19</t>
+  </si>
+  <si>
     <t>Miami Dade</t>
   </si>
   <si>
@@ -238,9 +265,6 @@
   </si>
   <si>
     <t>Use email for building department</t>
-  </si>
-  <si>
-    <t>2025-08-11</t>
   </si>
   <si>
     <t>Miami-Dade RER — Development Services &amp; Zoning</t>
@@ -334,9 +358,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11.0"/>
@@ -417,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -427,14 +448,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
@@ -955,8 +975,8 @@
       <c r="J9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="5">
-        <v>45880.0</v>
+      <c r="K9" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10">
@@ -964,31 +984,31 @@
         <v>36</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="5">
-        <v>45880.0</v>
+      <c r="K10" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -996,31 +1016,31 @@
         <v>36</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="5">
-        <v>45880.0</v>
+      <c r="K11" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -1028,31 +1048,31 @@
         <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="5">
-        <v>45880.0</v>
+      <c r="K12" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -1060,164 +1080,164 @@
         <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="5">
-        <v>45880.0</v>
+      <c r="K13" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="8">
-        <v>45880.0</v>
+      <c r="K14" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="8">
-        <v>45880.0</v>
+      <c r="K15" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="8">
-        <v>45880.0</v>
+      <c r="K16" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="8">
-        <v>45880.0</v>
+      <c r="K17" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>37</v>
@@ -1226,31 +1246,31 @@
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="G18" s="8"/>
       <c r="H18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
@@ -1259,31 +1279,31 @@
         <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="G19" s="8"/>
       <c r="H19" s="6" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
@@ -1292,31 +1312,31 @@
         <v>27</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="9"/>
+        <v>90</v>
+      </c>
+      <c r="G20" s="8"/>
       <c r="H20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>37</v>
@@ -1325,176 +1345,176 @@
         <v>32</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J25" s="11" t="s">
+      <c r="D25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K25" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
+      <c r="K25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
added project type with templates
</commit_message>
<xml_diff>
--- a/data/master.xlsx
+++ b/data/master.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="U4phjW+9dW+PlHYo8/jcYdho+MQ//z2yZfLsle8YJpM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Zd3IBcznrsg183IXPLA7COkIkWM73iIKRpokv/eC6b4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="132">
   <si>
     <t>County</t>
   </si>
@@ -126,6 +126,48 @@
     <t>fire@rivierabeach.org</t>
   </si>
   <si>
+    <t>Boynton Beach</t>
+  </si>
+  <si>
+    <t>Boynton Beach Building Division</t>
+  </si>
+  <si>
+    <t>https://boyntonbeachfl.mycusthelp.com/WEBAPP/_rs/(S(grztt2kh4fy0zchy4lqoj4oa))/RequestOpen.aspx?rqst=66</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Select Building Divison</t>
+  </si>
+  <si>
+    <t>2025-08-18</t>
+  </si>
+  <si>
+    <t>Boynton Beach Planning &amp; Zoning</t>
+  </si>
+  <si>
+    <t>Select Planning &amp; Zoning</t>
+  </si>
+  <si>
+    <t>Florida Department Of Health</t>
+  </si>
+  <si>
+    <t>https://fdh.mycusthelp.com/WEBAPP/_rs/(S(4aqjv0r34jlcqkt3cmwex033))/SupportHome.aspx?sSessionID=206170212118JIQMTBSSGWRDVANRIWFAXGJXHY[I</t>
+  </si>
+  <si>
+    <t>FDH Portal</t>
+  </si>
+  <si>
+    <t>Use Environmental Email Template</t>
+  </si>
+  <si>
+    <t>Boynton Beach Fire Rescue</t>
+  </si>
+  <si>
+    <t>Select Fire Rescue</t>
+  </si>
+  <si>
     <t>Lee</t>
   </si>
   <si>
@@ -189,9 +231,6 @@
     <t>https://fortmyers.mycusthelp.com/WEBAPP/_rs/(S(bydyqdkq3a4x5w4hxftxzzro))/RequestLogin.aspx?sSessionID=&amp;rqst=30&amp;target=ZwpfxNlipoMF2Ut+o/ukfVBzG+KwiVYui6tQ4jBaoyEbXnRUsppuaM9gxkGUAiqmY6bx2x6s+8GPrd0Llw+EPhizz6Hs8jVNfkAsIs+6AqG0aZ9sL0tMHkEdYrKJLPUVZ+7kk+92n5wQ/f/lJbyGLQ==</t>
   </si>
   <si>
-    <t>Portal</t>
-  </si>
-  <si>
     <t>Use portal + All-in-one email</t>
   </si>
   <si>
@@ -243,9 +282,6 @@
     <t>Monroe County Environmental Department</t>
   </si>
   <si>
-    <t>2025-08-18</t>
-  </si>
-  <si>
     <t>Monroe County Fire Department</t>
   </si>
   <si>
@@ -345,9 +381,6 @@
     <t>Public records portal; City Clerk is custodian</t>
   </si>
   <si>
-    <t>Florida Department Of Health</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -378,14 +411,14 @@
     <t>City of Miami Lakes - Environmental Department</t>
   </si>
   <si>
-    <t>d</t>
+    <t>Portal (Select Other)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -407,6 +440,19 @@
       <sz val="11.0"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -471,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -480,27 +526,36 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -891,780 +946,894 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="2" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>53</v>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="G10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>59</v>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>58</v>
+      <c r="G11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>61</v>
+      <c r="K11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>58</v>
+      <c r="I13" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>65</v>
+      <c r="K13" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="H15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K15" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="J16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="6" t="s">
+      <c r="D19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="K19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="6" t="s">
+      <c r="D20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="K20" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="6" t="s">
+      <c r="D21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="K21" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="6" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>78</v>
+      <c r="A23" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>78</v>
+      <c r="A24" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="3" t="s">
+      <c r="D24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="G24" s="11"/>
+      <c r="H24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="H26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="2" t="s">
         <v>116</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>75</v>
+      <c r="K26" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>111</v>
+      <c r="A27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="H27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>118</v>
+      <c r="I27" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>75</v>
+      <c r="K27" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="D28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="H28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+      <c r="K28" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
@@ -2641,33 +2810,41 @@
     <row r="1010" ht="15.75" customHeight="1"/>
     <row r="1011" ht="15.75" customHeight="1"/>
     <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2"/>
     <hyperlink r:id="rId2" ref="G3"/>
     <hyperlink r:id="rId3" ref="G6"/>
     <hyperlink r:id="rId4" ref="G7"/>
-    <hyperlink r:id="rId5" ref="G9"/>
-    <hyperlink r:id="rId6" ref="G10"/>
-    <hyperlink r:id="rId7" ref="G11"/>
-    <hyperlink r:id="rId8" ref="G12"/>
+    <hyperlink r:id="rId5" ref="G8"/>
+    <hyperlink r:id="rId6" ref="G9"/>
+    <hyperlink r:id="rId7" ref="G10"/>
+    <hyperlink r:id="rId8" ref="G11"/>
     <hyperlink r:id="rId9" ref="G13"/>
     <hyperlink r:id="rId10" ref="G14"/>
     <hyperlink r:id="rId11" ref="G15"/>
     <hyperlink r:id="rId12" ref="G16"/>
     <hyperlink r:id="rId13" ref="G17"/>
-    <hyperlink r:id="rId14" ref="G21"/>
-    <hyperlink r:id="rId15" ref="G22"/>
-    <hyperlink r:id="rId16" ref="G23"/>
-    <hyperlink r:id="rId17" ref="G24"/>
+    <hyperlink r:id="rId14" ref="G18"/>
+    <hyperlink r:id="rId15" ref="G19"/>
+    <hyperlink r:id="rId16" ref="G20"/>
+    <hyperlink r:id="rId17" ref="G21"/>
     <hyperlink r:id="rId18" ref="G25"/>
     <hyperlink r:id="rId19" ref="G26"/>
     <hyperlink r:id="rId20" ref="G27"/>
     <hyperlink r:id="rId21" ref="G28"/>
+    <hyperlink r:id="rId22" ref="G29"/>
+    <hyperlink r:id="rId23" ref="G30"/>
+    <hyperlink r:id="rId24" ref="G31"/>
+    <hyperlink r:id="rId25" ref="G32"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId22"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>